<commit_message>
Finalização da atualização de versão de desenvolvimento para produção
</commit_message>
<xml_diff>
--- a/docs/planilhas/Prototipo - 52 Semanas.xlsx
+++ b/docs/planilhas/Prototipo - 52 Semanas.xlsx
@@ -13,21 +13,11 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
   <authors>
-    <author>tc={de8ae49a-2fda-4934-b086-ad567182a36b}</author>
-    <author>tc={fbcdd032-f91e-4f46-ab3b-25fa6add870e}</author>
+    <author>tc={11e71ae3-26b5-4bff-aa10-88fe9c594959}</author>
+    <author>tc={d39a8dd3-abec-4c08-ae92-0865594ff71d}</author>
   </authors>
   <commentList>
-    <comment authorId="0" xr:uid="{de8ae49a-2fda-4934-b086-ad567182a36b}" ref="C5">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
- Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-	Valor base semanal: define o ritmo do desafio das 52 semanas.
-Exemplo: se o valor base for R$ 5, na semana 1 você investe R$ 5, na semana 2 R$ 10, na semana 3 R$ 15… até o final do ciclo.
-</t>
-      </text>
-    </comment>
-    <comment authorId="1" xr:uid="{fbcdd032-f91e-4f46-ab3b-25fa6add870e}" ref="H24">
+    <comment authorId="0" xr:uid="{11e71ae3-26b5-4bff-aa10-88fe9c594959}" ref="H24">
       <text>
         <t xml:space="preserve">[Threaded comment]
  Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -41,12 +31,22 @@
 </t>
       </text>
     </comment>
+    <comment authorId="1" xr:uid="{d39a8dd3-abec-4c08-ae92-0865594ff71d}" ref="C5">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+ Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+	Valor base semanal: define o ritmo do desafio das 52 semanas.
+Exemplo: se o valor base for R$ 5, na semana 1 você investe R$ 5, na semana 2 R$ 10, na semana 3 R$ 15… até o final do ciclo.
+</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Prototipo - 52 Semanas</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>ANALISE</t>
+  </si>
+  <si>
+    <t>DESAFIO DAS 52 SEMANAS I Veja como funciona!</t>
   </si>
   <si>
     <t>Coluna</t>
@@ -118,7 +121,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$R$ -416]#,##0.00"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -143,6 +146,12 @@
       <name val="Times New Roman"/>
     </font>
     <font/>
+    <font>
+      <u/>
+      <sz val="12.0"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -335,7 +344,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -359,6 +368,9 @@
     </xf>
     <xf borderId="2" fillId="3" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="3" fillId="3" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="4" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
@@ -457,7 +469,7 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <x18tc:personList xmlns:x18tc="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments">
-  <x18tc:person displayName="Arthur Paes Leme Stiegler" id="{a2e796bd-1c21-474a-b280-f5d863e3155b}" providerId="google-sheets"/>
+  <x18tc:person displayName="Arthur Paes Leme Stiegler" id="{f5af2723-c3f9-4cf6-865d-6f16396a6e8e}" providerId="google-sheets"/>
 </x18tc:personList>
 </file>
 
@@ -657,11 +669,11 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <x18tc:ThreadedComments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x18tc="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <x18tc:threadedComment ref="C5" dT="2026-01-26T02:17:19.00" personId="{a2e796bd-1c21-474a-b280-f5d863e3155b}" id="{de8ae49a-2fda-4934-b086-ad567182a36b}" done="0">
+  <x18tc:threadedComment ref="C5" dT="2026-01-26T02:17:19.00" personId="{f5af2723-c3f9-4cf6-865d-6f16396a6e8e}" id="{d39a8dd3-abec-4c08-ae92-0865594ff71d}" done="0">
     <x18tc:text xml:space="preserve">Valor base semanal: define o ritmo do desafio das 52 semanas.
 Exemplo: se o valor base for R$ 5, na semana 1 você investe R$ 5, na semana 2 R$ 10, na semana 3 R$ 15… até o final do ciclo.</x18tc:text>
   </x18tc:threadedComment>
-  <x18tc:threadedComment ref="H24" dT="2026-01-26T02:10:25.00" personId="{a2e796bd-1c21-474a-b280-f5d863e3155b}" id="{fbcdd032-f91e-4f46-ab3b-25fa6add870e}" done="0">
+  <x18tc:threadedComment ref="H24" dT="2026-01-26T02:10:25.00" personId="{f5af2723-c3f9-4cf6-865d-6f16396a6e8e}" id="{11e71ae3-26b5-4bff-aa10-88fe9c594959}" done="0">
     <x18tc:text xml:space="preserve">ℹ️ Por que aparece um 13º mês?
 Este planejamento considera que cada mês tem 4 semanas.
 Como o ano possui 52 semanas, ao dividir por 4 temos:
@@ -688,6 +700,7 @@
     <col customWidth="1" min="5" max="5" width="14.75"/>
     <col customWidth="1" min="6" max="6" width="16.75"/>
     <col customWidth="1" min="9" max="9" width="16.0"/>
+    <col customWidth="1" min="11" max="11" width="45.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -758,9 +771,10 @@
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
       <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
+      <c r="K3" s="9" t="s">
+        <v>3</v>
+      </c>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
@@ -781,20 +795,20 @@
     </row>
     <row r="4" ht="29.25" customHeight="1">
       <c r="A4" s="5"/>
-      <c r="B4" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="10" t="s">
+      <c r="B4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="C4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="9" t="s">
+      <c r="D4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="12">
+      <c r="E4" s="3"/>
+      <c r="F4" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="13">
         <f>SUMIF(F12:F63, TRUE, C12:D63)
  + SUMIF(F12:F63, TRUE, E12:E63)
 </f>
@@ -824,20 +838,20 @@
     </row>
     <row r="5" ht="40.5" customHeight="1">
       <c r="A5" s="5"/>
-      <c r="B5" s="13" t="s">
-        <v>7</v>
+      <c r="B5" s="14" t="s">
+        <v>8</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="15">
         <v>5.0</v>
       </c>
-      <c r="D5" s="15" t="s">
-        <v>8</v>
+      <c r="D5" s="16" t="s">
+        <v>9</v>
       </c>
       <c r="E5" s="3"/>
-      <c r="F5" s="16" t="s">
-        <v>9</v>
+      <c r="F5" s="17" t="s">
+        <v>10</v>
       </c>
-      <c r="G5" s="17">
+      <c r="G5" s="18">
         <f>SUMIF(F12:F63, TRUE, C12:C63) / SUM(C12:C63)
 </f>
         <v>0.0007256894049</v>
@@ -866,15 +880,15 @@
     </row>
     <row r="6" ht="24.0" customHeight="1">
       <c r="A6" s="5"/>
-      <c r="B6" s="18" t="s">
-        <v>10</v>
+      <c r="B6" s="19" t="s">
+        <v>11</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="20">
         <f> C5 * 1378</f>
         <v>6890</v>
       </c>
-      <c r="D6" s="20" t="s">
-        <v>11</v>
+      <c r="D6" s="21" t="s">
+        <v>12</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -994,7 +1008,7 @@
     <row r="10">
       <c r="A10" s="5"/>
       <c r="B10" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -1002,7 +1016,7 @@
       <c r="F10" s="8"/>
       <c r="G10" s="3"/>
       <c r="H10" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I10" s="8"/>
       <c r="J10" s="3"/>
@@ -1027,27 +1041,27 @@
     </row>
     <row r="11">
       <c r="A11" s="5"/>
-      <c r="B11" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="10" t="s">
+      <c r="B11" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="C11" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="D11" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="E11" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="9" t="s">
+      <c r="F11" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="I11" s="11" t="s">
+      <c r="G11" s="3"/>
+      <c r="H11" s="10" t="s">
         <v>20</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>21</v>
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -1071,28 +1085,28 @@
     </row>
     <row r="12">
       <c r="A12" s="5"/>
-      <c r="B12" s="13">
+      <c r="B12" s="14">
         <v>1.0</v>
       </c>
-      <c r="C12" s="21">
+      <c r="C12" s="22">
         <f t="shared" ref="C12:C63" si="1"> ($C$5 * B12)</f>
         <v>5</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="22">
         <f> ($C$5 * B12)</f>
         <v>5</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="15">
         <v>0.0</v>
       </c>
-      <c r="F12" s="15" t="b">
+      <c r="F12" s="16" t="b">
         <v>1</v>
       </c>
       <c r="G12" s="3"/>
-      <c r="H12" s="13">
+      <c r="H12" s="14">
         <v>1.0</v>
       </c>
-      <c r="I12" s="22">
+      <c r="I12" s="23">
         <f t="shared" ref="I12:I24" si="2">SUMIFS($C$12:$C$63, $B$12:$B$63, "&gt;="&amp;((H12-1)*4+1), $B$12:$B$63, "&lt;="&amp;(H12*4))
 </f>
         <v>50</v>
@@ -1119,28 +1133,28 @@
     </row>
     <row r="13">
       <c r="A13" s="5"/>
-      <c r="B13" s="23">
+      <c r="B13" s="24">
         <v>2.0</v>
       </c>
-      <c r="C13" s="24">
+      <c r="C13" s="25">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="D13" s="24">
+      <c r="D13" s="25">
         <f t="shared" ref="D13:D63" si="3"> D12 + C13</f>
         <v>15</v>
       </c>
-      <c r="E13" s="25">
+      <c r="E13" s="26">
         <v>0.0</v>
       </c>
-      <c r="F13" s="26" t="b">
+      <c r="F13" s="27" t="b">
         <v>0</v>
       </c>
       <c r="G13" s="3"/>
-      <c r="H13" s="23">
+      <c r="H13" s="24">
         <v>2.0</v>
       </c>
-      <c r="I13" s="27">
+      <c r="I13" s="28">
         <f t="shared" si="2"/>
         <v>130</v>
       </c>
@@ -1166,28 +1180,28 @@
     </row>
     <row r="14">
       <c r="A14" s="5"/>
-      <c r="B14" s="13">
+      <c r="B14" s="14">
         <v>3.0</v>
       </c>
-      <c r="C14" s="21">
+      <c r="C14" s="22">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="D14" s="21">
+      <c r="D14" s="22">
         <f t="shared" si="3"/>
         <v>30</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="15">
         <v>0.0</v>
       </c>
-      <c r="F14" s="15" t="b">
+      <c r="F14" s="16" t="b">
         <v>0</v>
       </c>
       <c r="G14" s="3"/>
-      <c r="H14" s="13">
+      <c r="H14" s="14">
         <v>3.0</v>
       </c>
-      <c r="I14" s="22">
+      <c r="I14" s="23">
         <f t="shared" si="2"/>
         <v>210</v>
       </c>
@@ -1213,28 +1227,28 @@
     </row>
     <row r="15">
       <c r="A15" s="5"/>
-      <c r="B15" s="23">
+      <c r="B15" s="24">
         <v>4.0</v>
       </c>
-      <c r="C15" s="24">
+      <c r="C15" s="25">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="D15" s="24">
+      <c r="D15" s="25">
         <f t="shared" si="3"/>
         <v>50</v>
       </c>
-      <c r="E15" s="25">
+      <c r="E15" s="26">
         <v>0.0</v>
       </c>
-      <c r="F15" s="26" t="b">
+      <c r="F15" s="27" t="b">
         <v>0</v>
       </c>
       <c r="G15" s="3"/>
-      <c r="H15" s="23">
+      <c r="H15" s="24">
         <v>4.0</v>
       </c>
-      <c r="I15" s="27">
+      <c r="I15" s="28">
         <f t="shared" si="2"/>
         <v>290</v>
       </c>
@@ -1260,28 +1274,28 @@
     </row>
     <row r="16">
       <c r="A16" s="5"/>
-      <c r="B16" s="13">
+      <c r="B16" s="14">
         <v>5.0</v>
       </c>
-      <c r="C16" s="21">
+      <c r="C16" s="22">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="D16" s="21">
+      <c r="D16" s="22">
         <f t="shared" si="3"/>
         <v>75</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="15">
         <v>0.0</v>
       </c>
-      <c r="F16" s="15" t="b">
+      <c r="F16" s="16" t="b">
         <v>0</v>
       </c>
       <c r="G16" s="3"/>
-      <c r="H16" s="13">
+      <c r="H16" s="14">
         <v>5.0</v>
       </c>
-      <c r="I16" s="22">
+      <c r="I16" s="23">
         <f t="shared" si="2"/>
         <v>370</v>
       </c>
@@ -1307,28 +1321,28 @@
     </row>
     <row r="17">
       <c r="A17" s="5"/>
-      <c r="B17" s="23">
+      <c r="B17" s="24">
         <v>6.0</v>
       </c>
-      <c r="C17" s="24">
+      <c r="C17" s="25">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="D17" s="24">
+      <c r="D17" s="25">
         <f t="shared" si="3"/>
         <v>105</v>
       </c>
-      <c r="E17" s="25">
+      <c r="E17" s="26">
         <v>0.0</v>
       </c>
-      <c r="F17" s="27" t="b">
+      <c r="F17" s="28" t="b">
         <v>0</v>
       </c>
       <c r="G17" s="3"/>
-      <c r="H17" s="23">
+      <c r="H17" s="24">
         <v>6.0</v>
       </c>
-      <c r="I17" s="27">
+      <c r="I17" s="28">
         <f t="shared" si="2"/>
         <v>450</v>
       </c>
@@ -1354,28 +1368,28 @@
     </row>
     <row r="18">
       <c r="A18" s="5"/>
-      <c r="B18" s="13">
+      <c r="B18" s="14">
         <v>7.0</v>
       </c>
-      <c r="C18" s="21">
+      <c r="C18" s="22">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="D18" s="21">
+      <c r="D18" s="22">
         <f t="shared" si="3"/>
         <v>140</v>
       </c>
-      <c r="E18" s="14">
+      <c r="E18" s="15">
         <v>0.0</v>
       </c>
-      <c r="F18" s="22" t="b">
+      <c r="F18" s="23" t="b">
         <v>0</v>
       </c>
       <c r="G18" s="3"/>
-      <c r="H18" s="13">
+      <c r="H18" s="14">
         <v>7.0</v>
       </c>
-      <c r="I18" s="22">
+      <c r="I18" s="23">
         <f t="shared" si="2"/>
         <v>530</v>
       </c>
@@ -1401,28 +1415,28 @@
     </row>
     <row r="19">
       <c r="A19" s="5"/>
-      <c r="B19" s="23">
+      <c r="B19" s="24">
         <v>8.0</v>
       </c>
-      <c r="C19" s="24">
+      <c r="C19" s="25">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="D19" s="24">
+      <c r="D19" s="25">
         <f t="shared" si="3"/>
         <v>180</v>
       </c>
-      <c r="E19" s="25">
+      <c r="E19" s="26">
         <v>0.0</v>
       </c>
-      <c r="F19" s="27" t="b">
+      <c r="F19" s="28" t="b">
         <v>0</v>
       </c>
       <c r="G19" s="3"/>
-      <c r="H19" s="23">
+      <c r="H19" s="24">
         <v>8.0</v>
       </c>
-      <c r="I19" s="27">
+      <c r="I19" s="28">
         <f t="shared" si="2"/>
         <v>610</v>
       </c>
@@ -1448,28 +1462,28 @@
     </row>
     <row r="20">
       <c r="A20" s="5"/>
-      <c r="B20" s="13">
+      <c r="B20" s="14">
         <v>9.0</v>
       </c>
-      <c r="C20" s="21">
+      <c r="C20" s="22">
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="D20" s="21">
+      <c r="D20" s="22">
         <f t="shared" si="3"/>
         <v>225</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E20" s="15">
         <v>0.0</v>
       </c>
-      <c r="F20" s="22" t="b">
+      <c r="F20" s="23" t="b">
         <v>0</v>
       </c>
       <c r="G20" s="3"/>
-      <c r="H20" s="13">
+      <c r="H20" s="14">
         <v>9.0</v>
       </c>
-      <c r="I20" s="22">
+      <c r="I20" s="23">
         <f t="shared" si="2"/>
         <v>690</v>
       </c>
@@ -1495,28 +1509,28 @@
     </row>
     <row r="21">
       <c r="A21" s="5"/>
-      <c r="B21" s="23">
+      <c r="B21" s="24">
         <v>10.0</v>
       </c>
-      <c r="C21" s="24">
+      <c r="C21" s="25">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="D21" s="24">
+      <c r="D21" s="25">
         <f t="shared" si="3"/>
         <v>275</v>
       </c>
-      <c r="E21" s="25">
+      <c r="E21" s="26">
         <v>0.0</v>
       </c>
-      <c r="F21" s="27" t="b">
+      <c r="F21" s="28" t="b">
         <v>0</v>
       </c>
       <c r="G21" s="3"/>
-      <c r="H21" s="23">
+      <c r="H21" s="24">
         <v>10.0</v>
       </c>
-      <c r="I21" s="27">
+      <c r="I21" s="28">
         <f t="shared" si="2"/>
         <v>770</v>
       </c>
@@ -1542,28 +1556,28 @@
     </row>
     <row r="22">
       <c r="A22" s="5"/>
-      <c r="B22" s="13">
+      <c r="B22" s="14">
         <v>11.0</v>
       </c>
-      <c r="C22" s="21">
+      <c r="C22" s="22">
         <f t="shared" si="1"/>
         <v>55</v>
       </c>
-      <c r="D22" s="21">
+      <c r="D22" s="22">
         <f t="shared" si="3"/>
         <v>330</v>
       </c>
-      <c r="E22" s="14">
+      <c r="E22" s="15">
         <v>0.0</v>
       </c>
-      <c r="F22" s="22" t="b">
+      <c r="F22" s="23" t="b">
         <v>0</v>
       </c>
       <c r="G22" s="3"/>
-      <c r="H22" s="13">
+      <c r="H22" s="14">
         <v>11.0</v>
       </c>
-      <c r="I22" s="22">
+      <c r="I22" s="23">
         <f t="shared" si="2"/>
         <v>850</v>
       </c>
@@ -1589,28 +1603,28 @@
     </row>
     <row r="23">
       <c r="A23" s="5"/>
-      <c r="B23" s="23">
+      <c r="B23" s="24">
         <v>12.0</v>
       </c>
-      <c r="C23" s="24">
+      <c r="C23" s="25">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="D23" s="24">
+      <c r="D23" s="25">
         <f t="shared" si="3"/>
         <v>390</v>
       </c>
-      <c r="E23" s="25">
+      <c r="E23" s="26">
         <v>0.0</v>
       </c>
-      <c r="F23" s="27" t="b">
+      <c r="F23" s="28" t="b">
         <v>0</v>
       </c>
       <c r="G23" s="3"/>
-      <c r="H23" s="23">
+      <c r="H23" s="24">
         <v>12.0</v>
       </c>
-      <c r="I23" s="27">
+      <c r="I23" s="28">
         <f t="shared" si="2"/>
         <v>930</v>
       </c>
@@ -1636,28 +1650,28 @@
     </row>
     <row r="24">
       <c r="A24" s="5"/>
-      <c r="B24" s="13">
+      <c r="B24" s="14">
         <v>13.0</v>
       </c>
-      <c r="C24" s="21">
+      <c r="C24" s="22">
         <f t="shared" si="1"/>
         <v>65</v>
       </c>
-      <c r="D24" s="21">
+      <c r="D24" s="22">
         <f t="shared" si="3"/>
         <v>455</v>
       </c>
-      <c r="E24" s="14">
+      <c r="E24" s="15">
         <v>0.0</v>
       </c>
-      <c r="F24" s="22" t="b">
+      <c r="F24" s="23" t="b">
         <v>0</v>
       </c>
       <c r="G24" s="3"/>
-      <c r="H24" s="16">
+      <c r="H24" s="17">
         <v>13.0</v>
       </c>
-      <c r="I24" s="28">
+      <c r="I24" s="29">
         <f t="shared" si="2"/>
         <v>1010</v>
       </c>
@@ -1683,21 +1697,21 @@
     </row>
     <row r="25">
       <c r="A25" s="5"/>
-      <c r="B25" s="23">
+      <c r="B25" s="24">
         <v>14.0</v>
       </c>
-      <c r="C25" s="24">
+      <c r="C25" s="25">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
-      <c r="D25" s="24">
+      <c r="D25" s="25">
         <f t="shared" si="3"/>
         <v>525</v>
       </c>
-      <c r="E25" s="25">
+      <c r="E25" s="26">
         <v>0.0</v>
       </c>
-      <c r="F25" s="27" t="b">
+      <c r="F25" s="28" t="b">
         <v>0</v>
       </c>
       <c r="G25" s="3"/>
@@ -1725,21 +1739,21 @@
     </row>
     <row r="26">
       <c r="A26" s="5"/>
-      <c r="B26" s="13">
+      <c r="B26" s="14">
         <v>15.0</v>
       </c>
-      <c r="C26" s="21">
+      <c r="C26" s="22">
         <f t="shared" si="1"/>
         <v>75</v>
       </c>
-      <c r="D26" s="21">
+      <c r="D26" s="22">
         <f t="shared" si="3"/>
         <v>600</v>
       </c>
-      <c r="E26" s="14">
+      <c r="E26" s="15">
         <v>0.0</v>
       </c>
-      <c r="F26" s="22" t="b">
+      <c r="F26" s="23" t="b">
         <v>0</v>
       </c>
       <c r="G26" s="3"/>
@@ -1767,21 +1781,21 @@
     </row>
     <row r="27">
       <c r="A27" s="5"/>
-      <c r="B27" s="23">
+      <c r="B27" s="24">
         <v>16.0</v>
       </c>
-      <c r="C27" s="24">
+      <c r="C27" s="25">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="D27" s="24">
+      <c r="D27" s="25">
         <f t="shared" si="3"/>
         <v>680</v>
       </c>
-      <c r="E27" s="25">
+      <c r="E27" s="26">
         <v>0.0</v>
       </c>
-      <c r="F27" s="27" t="b">
+      <c r="F27" s="28" t="b">
         <v>0</v>
       </c>
       <c r="G27" s="3"/>
@@ -1809,21 +1823,21 @@
     </row>
     <row r="28">
       <c r="A28" s="5"/>
-      <c r="B28" s="13">
+      <c r="B28" s="14">
         <v>17.0</v>
       </c>
-      <c r="C28" s="21">
+      <c r="C28" s="22">
         <f t="shared" si="1"/>
         <v>85</v>
       </c>
-      <c r="D28" s="21">
+      <c r="D28" s="22">
         <f t="shared" si="3"/>
         <v>765</v>
       </c>
-      <c r="E28" s="14">
+      <c r="E28" s="15">
         <v>0.0</v>
       </c>
-      <c r="F28" s="22" t="b">
+      <c r="F28" s="23" t="b">
         <v>0</v>
       </c>
       <c r="G28" s="3"/>
@@ -1851,21 +1865,21 @@
     </row>
     <row r="29">
       <c r="A29" s="5"/>
-      <c r="B29" s="23">
+      <c r="B29" s="24">
         <v>18.0</v>
       </c>
-      <c r="C29" s="24">
+      <c r="C29" s="25">
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
-      <c r="D29" s="24">
+      <c r="D29" s="25">
         <f t="shared" si="3"/>
         <v>855</v>
       </c>
-      <c r="E29" s="25">
+      <c r="E29" s="26">
         <v>0.0</v>
       </c>
-      <c r="F29" s="27" t="b">
+      <c r="F29" s="28" t="b">
         <v>0</v>
       </c>
       <c r="G29" s="3"/>
@@ -1893,21 +1907,21 @@
     </row>
     <row r="30">
       <c r="A30" s="5"/>
-      <c r="B30" s="13">
+      <c r="B30" s="14">
         <v>19.0</v>
       </c>
-      <c r="C30" s="21">
+      <c r="C30" s="22">
         <f t="shared" si="1"/>
         <v>95</v>
       </c>
-      <c r="D30" s="21">
+      <c r="D30" s="22">
         <f t="shared" si="3"/>
         <v>950</v>
       </c>
-      <c r="E30" s="14">
+      <c r="E30" s="15">
         <v>0.0</v>
       </c>
-      <c r="F30" s="22" t="b">
+      <c r="F30" s="23" t="b">
         <v>0</v>
       </c>
       <c r="G30" s="3"/>
@@ -1935,21 +1949,21 @@
     </row>
     <row r="31">
       <c r="A31" s="5"/>
-      <c r="B31" s="23">
+      <c r="B31" s="24">
         <v>20.0</v>
       </c>
-      <c r="C31" s="24">
+      <c r="C31" s="25">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="D31" s="24">
+      <c r="D31" s="25">
         <f t="shared" si="3"/>
         <v>1050</v>
       </c>
-      <c r="E31" s="25">
+      <c r="E31" s="26">
         <v>0.0</v>
       </c>
-      <c r="F31" s="27" t="b">
+      <c r="F31" s="28" t="b">
         <v>0</v>
       </c>
       <c r="G31" s="3"/>
@@ -1977,21 +1991,21 @@
     </row>
     <row r="32">
       <c r="A32" s="5"/>
-      <c r="B32" s="13">
+      <c r="B32" s="14">
         <v>21.0</v>
       </c>
-      <c r="C32" s="21">
+      <c r="C32" s="22">
         <f t="shared" si="1"/>
         <v>105</v>
       </c>
-      <c r="D32" s="21">
+      <c r="D32" s="22">
         <f t="shared" si="3"/>
         <v>1155</v>
       </c>
-      <c r="E32" s="14">
+      <c r="E32" s="15">
         <v>0.0</v>
       </c>
-      <c r="F32" s="22" t="b">
+      <c r="F32" s="23" t="b">
         <v>0</v>
       </c>
       <c r="G32" s="3"/>
@@ -2019,21 +2033,21 @@
     </row>
     <row r="33">
       <c r="A33" s="5"/>
-      <c r="B33" s="23">
+      <c r="B33" s="24">
         <v>22.0</v>
       </c>
-      <c r="C33" s="24">
+      <c r="C33" s="25">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="D33" s="24">
+      <c r="D33" s="25">
         <f t="shared" si="3"/>
         <v>1265</v>
       </c>
-      <c r="E33" s="25">
+      <c r="E33" s="26">
         <v>0.0</v>
       </c>
-      <c r="F33" s="27" t="b">
+      <c r="F33" s="28" t="b">
         <v>0</v>
       </c>
       <c r="G33" s="3"/>
@@ -2061,21 +2075,21 @@
     </row>
     <row r="34">
       <c r="A34" s="5"/>
-      <c r="B34" s="13">
+      <c r="B34" s="14">
         <v>23.0</v>
       </c>
-      <c r="C34" s="21">
+      <c r="C34" s="22">
         <f t="shared" si="1"/>
         <v>115</v>
       </c>
-      <c r="D34" s="21">
+      <c r="D34" s="22">
         <f t="shared" si="3"/>
         <v>1380</v>
       </c>
-      <c r="E34" s="14">
+      <c r="E34" s="15">
         <v>0.0</v>
       </c>
-      <c r="F34" s="22" t="b">
+      <c r="F34" s="23" t="b">
         <v>0</v>
       </c>
       <c r="G34" s="3"/>
@@ -2103,21 +2117,21 @@
     </row>
     <row r="35">
       <c r="A35" s="5"/>
-      <c r="B35" s="23">
+      <c r="B35" s="24">
         <v>24.0</v>
       </c>
-      <c r="C35" s="24">
+      <c r="C35" s="25">
         <f t="shared" si="1"/>
         <v>120</v>
       </c>
-      <c r="D35" s="24">
+      <c r="D35" s="25">
         <f t="shared" si="3"/>
         <v>1500</v>
       </c>
-      <c r="E35" s="25">
+      <c r="E35" s="26">
         <v>0.0</v>
       </c>
-      <c r="F35" s="27" t="b">
+      <c r="F35" s="28" t="b">
         <v>0</v>
       </c>
       <c r="G35" s="3"/>
@@ -2145,21 +2159,21 @@
     </row>
     <row r="36">
       <c r="A36" s="5"/>
-      <c r="B36" s="13">
+      <c r="B36" s="14">
         <v>25.0</v>
       </c>
-      <c r="C36" s="21">
+      <c r="C36" s="22">
         <f t="shared" si="1"/>
         <v>125</v>
       </c>
-      <c r="D36" s="21">
+      <c r="D36" s="22">
         <f t="shared" si="3"/>
         <v>1625</v>
       </c>
-      <c r="E36" s="14">
+      <c r="E36" s="15">
         <v>0.0</v>
       </c>
-      <c r="F36" s="22" t="b">
+      <c r="F36" s="23" t="b">
         <v>0</v>
       </c>
       <c r="G36" s="3"/>
@@ -2187,21 +2201,21 @@
     </row>
     <row r="37">
       <c r="A37" s="5"/>
-      <c r="B37" s="23">
+      <c r="B37" s="24">
         <v>26.0</v>
       </c>
-      <c r="C37" s="24">
+      <c r="C37" s="25">
         <f t="shared" si="1"/>
         <v>130</v>
       </c>
-      <c r="D37" s="24">
+      <c r="D37" s="25">
         <f t="shared" si="3"/>
         <v>1755</v>
       </c>
-      <c r="E37" s="25">
+      <c r="E37" s="26">
         <v>0.0</v>
       </c>
-      <c r="F37" s="27" t="b">
+      <c r="F37" s="28" t="b">
         <v>0</v>
       </c>
       <c r="G37" s="3"/>
@@ -2229,21 +2243,21 @@
     </row>
     <row r="38">
       <c r="A38" s="5"/>
-      <c r="B38" s="13">
+      <c r="B38" s="14">
         <v>27.0</v>
       </c>
-      <c r="C38" s="21">
+      <c r="C38" s="22">
         <f t="shared" si="1"/>
         <v>135</v>
       </c>
-      <c r="D38" s="21">
+      <c r="D38" s="22">
         <f t="shared" si="3"/>
         <v>1890</v>
       </c>
-      <c r="E38" s="14">
+      <c r="E38" s="15">
         <v>0.0</v>
       </c>
-      <c r="F38" s="22" t="b">
+      <c r="F38" s="23" t="b">
         <v>0</v>
       </c>
       <c r="G38" s="3"/>
@@ -2271,21 +2285,21 @@
     </row>
     <row r="39">
       <c r="A39" s="5"/>
-      <c r="B39" s="23">
+      <c r="B39" s="24">
         <v>28.0</v>
       </c>
-      <c r="C39" s="24">
+      <c r="C39" s="25">
         <f t="shared" si="1"/>
         <v>140</v>
       </c>
-      <c r="D39" s="24">
+      <c r="D39" s="25">
         <f t="shared" si="3"/>
         <v>2030</v>
       </c>
-      <c r="E39" s="25">
+      <c r="E39" s="26">
         <v>0.0</v>
       </c>
-      <c r="F39" s="27" t="b">
+      <c r="F39" s="28" t="b">
         <v>0</v>
       </c>
       <c r="G39" s="3"/>
@@ -2313,21 +2327,21 @@
     </row>
     <row r="40">
       <c r="A40" s="5"/>
-      <c r="B40" s="13">
+      <c r="B40" s="14">
         <v>29.0</v>
       </c>
-      <c r="C40" s="21">
+      <c r="C40" s="22">
         <f t="shared" si="1"/>
         <v>145</v>
       </c>
-      <c r="D40" s="21">
+      <c r="D40" s="22">
         <f t="shared" si="3"/>
         <v>2175</v>
       </c>
-      <c r="E40" s="14">
+      <c r="E40" s="15">
         <v>0.0</v>
       </c>
-      <c r="F40" s="22" t="b">
+      <c r="F40" s="23" t="b">
         <v>0</v>
       </c>
       <c r="G40" s="3"/>
@@ -2355,21 +2369,21 @@
     </row>
     <row r="41">
       <c r="A41" s="5"/>
-      <c r="B41" s="23">
+      <c r="B41" s="24">
         <v>30.0</v>
       </c>
-      <c r="C41" s="24">
+      <c r="C41" s="25">
         <f t="shared" si="1"/>
         <v>150</v>
       </c>
-      <c r="D41" s="24">
+      <c r="D41" s="25">
         <f t="shared" si="3"/>
         <v>2325</v>
       </c>
-      <c r="E41" s="25">
+      <c r="E41" s="26">
         <v>0.0</v>
       </c>
-      <c r="F41" s="27" t="b">
+      <c r="F41" s="28" t="b">
         <v>0</v>
       </c>
       <c r="G41" s="3"/>
@@ -2397,21 +2411,21 @@
     </row>
     <row r="42">
       <c r="A42" s="5"/>
-      <c r="B42" s="13">
+      <c r="B42" s="14">
         <v>31.0</v>
       </c>
-      <c r="C42" s="21">
+      <c r="C42" s="22">
         <f t="shared" si="1"/>
         <v>155</v>
       </c>
-      <c r="D42" s="21">
+      <c r="D42" s="22">
         <f t="shared" si="3"/>
         <v>2480</v>
       </c>
-      <c r="E42" s="14">
+      <c r="E42" s="15">
         <v>0.0</v>
       </c>
-      <c r="F42" s="22" t="b">
+      <c r="F42" s="23" t="b">
         <v>0</v>
       </c>
       <c r="G42" s="3"/>
@@ -2439,21 +2453,21 @@
     </row>
     <row r="43">
       <c r="A43" s="5"/>
-      <c r="B43" s="23">
+      <c r="B43" s="24">
         <v>32.0</v>
       </c>
-      <c r="C43" s="24">
+      <c r="C43" s="25">
         <f t="shared" si="1"/>
         <v>160</v>
       </c>
-      <c r="D43" s="24">
+      <c r="D43" s="25">
         <f t="shared" si="3"/>
         <v>2640</v>
       </c>
-      <c r="E43" s="25">
+      <c r="E43" s="26">
         <v>0.0</v>
       </c>
-      <c r="F43" s="27" t="b">
+      <c r="F43" s="28" t="b">
         <v>0</v>
       </c>
       <c r="G43" s="3"/>
@@ -2481,21 +2495,21 @@
     </row>
     <row r="44">
       <c r="A44" s="5"/>
-      <c r="B44" s="13">
+      <c r="B44" s="14">
         <v>33.0</v>
       </c>
-      <c r="C44" s="21">
+      <c r="C44" s="22">
         <f t="shared" si="1"/>
         <v>165</v>
       </c>
-      <c r="D44" s="21">
+      <c r="D44" s="22">
         <f t="shared" si="3"/>
         <v>2805</v>
       </c>
-      <c r="E44" s="14">
+      <c r="E44" s="15">
         <v>0.0</v>
       </c>
-      <c r="F44" s="22" t="b">
+      <c r="F44" s="23" t="b">
         <v>0</v>
       </c>
       <c r="G44" s="3"/>
@@ -2523,21 +2537,21 @@
     </row>
     <row r="45">
       <c r="A45" s="5"/>
-      <c r="B45" s="23">
+      <c r="B45" s="24">
         <v>34.0</v>
       </c>
-      <c r="C45" s="24">
+      <c r="C45" s="25">
         <f t="shared" si="1"/>
         <v>170</v>
       </c>
-      <c r="D45" s="24">
+      <c r="D45" s="25">
         <f t="shared" si="3"/>
         <v>2975</v>
       </c>
-      <c r="E45" s="25">
+      <c r="E45" s="26">
         <v>0.0</v>
       </c>
-      <c r="F45" s="27" t="b">
+      <c r="F45" s="28" t="b">
         <v>0</v>
       </c>
       <c r="G45" s="3"/>
@@ -2565,21 +2579,21 @@
     </row>
     <row r="46">
       <c r="A46" s="5"/>
-      <c r="B46" s="13">
+      <c r="B46" s="14">
         <v>35.0</v>
       </c>
-      <c r="C46" s="21">
+      <c r="C46" s="22">
         <f t="shared" si="1"/>
         <v>175</v>
       </c>
-      <c r="D46" s="21">
+      <c r="D46" s="22">
         <f t="shared" si="3"/>
         <v>3150</v>
       </c>
-      <c r="E46" s="14">
+      <c r="E46" s="15">
         <v>0.0</v>
       </c>
-      <c r="F46" s="22" t="b">
+      <c r="F46" s="23" t="b">
         <v>0</v>
       </c>
       <c r="G46" s="3"/>
@@ -2607,21 +2621,21 @@
     </row>
     <row r="47">
       <c r="A47" s="5"/>
-      <c r="B47" s="23">
+      <c r="B47" s="24">
         <v>36.0</v>
       </c>
-      <c r="C47" s="24">
+      <c r="C47" s="25">
         <f t="shared" si="1"/>
         <v>180</v>
       </c>
-      <c r="D47" s="24">
+      <c r="D47" s="25">
         <f t="shared" si="3"/>
         <v>3330</v>
       </c>
-      <c r="E47" s="25">
+      <c r="E47" s="26">
         <v>0.0</v>
       </c>
-      <c r="F47" s="27" t="b">
+      <c r="F47" s="28" t="b">
         <v>0</v>
       </c>
       <c r="G47" s="3"/>
@@ -2649,21 +2663,21 @@
     </row>
     <row r="48">
       <c r="A48" s="5"/>
-      <c r="B48" s="13">
+      <c r="B48" s="14">
         <v>37.0</v>
       </c>
-      <c r="C48" s="21">
+      <c r="C48" s="22">
         <f t="shared" si="1"/>
         <v>185</v>
       </c>
-      <c r="D48" s="21">
+      <c r="D48" s="22">
         <f t="shared" si="3"/>
         <v>3515</v>
       </c>
-      <c r="E48" s="14">
+      <c r="E48" s="15">
         <v>0.0</v>
       </c>
-      <c r="F48" s="22" t="b">
+      <c r="F48" s="23" t="b">
         <v>0</v>
       </c>
       <c r="G48" s="3"/>
@@ -2691,21 +2705,21 @@
     </row>
     <row r="49">
       <c r="A49" s="5"/>
-      <c r="B49" s="23">
+      <c r="B49" s="24">
         <v>38.0</v>
       </c>
-      <c r="C49" s="24">
+      <c r="C49" s="25">
         <f t="shared" si="1"/>
         <v>190</v>
       </c>
-      <c r="D49" s="24">
+      <c r="D49" s="25">
         <f t="shared" si="3"/>
         <v>3705</v>
       </c>
-      <c r="E49" s="25">
+      <c r="E49" s="26">
         <v>0.0</v>
       </c>
-      <c r="F49" s="27" t="b">
+      <c r="F49" s="28" t="b">
         <v>0</v>
       </c>
       <c r="G49" s="3"/>
@@ -2733,21 +2747,21 @@
     </row>
     <row r="50">
       <c r="A50" s="5"/>
-      <c r="B50" s="13">
+      <c r="B50" s="14">
         <v>39.0</v>
       </c>
-      <c r="C50" s="21">
+      <c r="C50" s="22">
         <f t="shared" si="1"/>
         <v>195</v>
       </c>
-      <c r="D50" s="21">
+      <c r="D50" s="22">
         <f t="shared" si="3"/>
         <v>3900</v>
       </c>
-      <c r="E50" s="14">
+      <c r="E50" s="15">
         <v>0.0</v>
       </c>
-      <c r="F50" s="22" t="b">
+      <c r="F50" s="23" t="b">
         <v>0</v>
       </c>
       <c r="G50" s="3"/>
@@ -2775,21 +2789,21 @@
     </row>
     <row r="51">
       <c r="A51" s="5"/>
-      <c r="B51" s="23">
+      <c r="B51" s="24">
         <v>40.0</v>
       </c>
-      <c r="C51" s="24">
+      <c r="C51" s="25">
         <f t="shared" si="1"/>
         <v>200</v>
       </c>
-      <c r="D51" s="24">
+      <c r="D51" s="25">
         <f t="shared" si="3"/>
         <v>4100</v>
       </c>
-      <c r="E51" s="25">
+      <c r="E51" s="26">
         <v>0.0</v>
       </c>
-      <c r="F51" s="27" t="b">
+      <c r="F51" s="28" t="b">
         <v>0</v>
       </c>
       <c r="G51" s="3"/>
@@ -2817,21 +2831,21 @@
     </row>
     <row r="52">
       <c r="A52" s="5"/>
-      <c r="B52" s="13">
+      <c r="B52" s="14">
         <v>41.0</v>
       </c>
-      <c r="C52" s="21">
+      <c r="C52" s="22">
         <f t="shared" si="1"/>
         <v>205</v>
       </c>
-      <c r="D52" s="21">
+      <c r="D52" s="22">
         <f t="shared" si="3"/>
         <v>4305</v>
       </c>
-      <c r="E52" s="14">
+      <c r="E52" s="15">
         <v>0.0</v>
       </c>
-      <c r="F52" s="22" t="b">
+      <c r="F52" s="23" t="b">
         <v>0</v>
       </c>
       <c r="G52" s="3"/>
@@ -2859,21 +2873,21 @@
     </row>
     <row r="53">
       <c r="A53" s="5"/>
-      <c r="B53" s="23">
+      <c r="B53" s="24">
         <v>42.0</v>
       </c>
-      <c r="C53" s="24">
+      <c r="C53" s="25">
         <f t="shared" si="1"/>
         <v>210</v>
       </c>
-      <c r="D53" s="24">
+      <c r="D53" s="25">
         <f t="shared" si="3"/>
         <v>4515</v>
       </c>
-      <c r="E53" s="25">
+      <c r="E53" s="26">
         <v>0.0</v>
       </c>
-      <c r="F53" s="27" t="b">
+      <c r="F53" s="28" t="b">
         <v>0</v>
       </c>
       <c r="G53" s="3"/>
@@ -2901,21 +2915,21 @@
     </row>
     <row r="54">
       <c r="A54" s="5"/>
-      <c r="B54" s="13">
+      <c r="B54" s="14">
         <v>43.0</v>
       </c>
-      <c r="C54" s="21">
+      <c r="C54" s="22">
         <f t="shared" si="1"/>
         <v>215</v>
       </c>
-      <c r="D54" s="21">
+      <c r="D54" s="22">
         <f t="shared" si="3"/>
         <v>4730</v>
       </c>
-      <c r="E54" s="14">
+      <c r="E54" s="15">
         <v>0.0</v>
       </c>
-      <c r="F54" s="22" t="b">
+      <c r="F54" s="23" t="b">
         <v>0</v>
       </c>
       <c r="G54" s="3"/>
@@ -2943,21 +2957,21 @@
     </row>
     <row r="55">
       <c r="A55" s="5"/>
-      <c r="B55" s="23">
+      <c r="B55" s="24">
         <v>44.0</v>
       </c>
-      <c r="C55" s="24">
+      <c r="C55" s="25">
         <f t="shared" si="1"/>
         <v>220</v>
       </c>
-      <c r="D55" s="24">
+      <c r="D55" s="25">
         <f t="shared" si="3"/>
         <v>4950</v>
       </c>
-      <c r="E55" s="25">
+      <c r="E55" s="26">
         <v>0.0</v>
       </c>
-      <c r="F55" s="27" t="b">
+      <c r="F55" s="28" t="b">
         <v>0</v>
       </c>
       <c r="G55" s="3"/>
@@ -2985,21 +2999,21 @@
     </row>
     <row r="56">
       <c r="A56" s="5"/>
-      <c r="B56" s="13">
+      <c r="B56" s="14">
         <v>45.0</v>
       </c>
-      <c r="C56" s="21">
+      <c r="C56" s="22">
         <f t="shared" si="1"/>
         <v>225</v>
       </c>
-      <c r="D56" s="21">
+      <c r="D56" s="22">
         <f t="shared" si="3"/>
         <v>5175</v>
       </c>
-      <c r="E56" s="14">
+      <c r="E56" s="15">
         <v>0.0</v>
       </c>
-      <c r="F56" s="22" t="b">
+      <c r="F56" s="23" t="b">
         <v>0</v>
       </c>
       <c r="G56" s="3"/>
@@ -3027,21 +3041,21 @@
     </row>
     <row r="57">
       <c r="A57" s="5"/>
-      <c r="B57" s="23">
+      <c r="B57" s="24">
         <v>46.0</v>
       </c>
-      <c r="C57" s="24">
+      <c r="C57" s="25">
         <f t="shared" si="1"/>
         <v>230</v>
       </c>
-      <c r="D57" s="24">
+      <c r="D57" s="25">
         <f t="shared" si="3"/>
         <v>5405</v>
       </c>
-      <c r="E57" s="25">
+      <c r="E57" s="26">
         <v>0.0</v>
       </c>
-      <c r="F57" s="27" t="b">
+      <c r="F57" s="28" t="b">
         <v>0</v>
       </c>
       <c r="G57" s="3"/>
@@ -3069,21 +3083,21 @@
     </row>
     <row r="58">
       <c r="A58" s="5"/>
-      <c r="B58" s="13">
+      <c r="B58" s="14">
         <v>47.0</v>
       </c>
-      <c r="C58" s="21">
+      <c r="C58" s="22">
         <f t="shared" si="1"/>
         <v>235</v>
       </c>
-      <c r="D58" s="21">
+      <c r="D58" s="22">
         <f t="shared" si="3"/>
         <v>5640</v>
       </c>
-      <c r="E58" s="14">
+      <c r="E58" s="15">
         <v>0.0</v>
       </c>
-      <c r="F58" s="22" t="b">
+      <c r="F58" s="23" t="b">
         <v>0</v>
       </c>
       <c r="G58" s="3"/>
@@ -3111,21 +3125,21 @@
     </row>
     <row r="59">
       <c r="A59" s="5"/>
-      <c r="B59" s="23">
+      <c r="B59" s="24">
         <v>48.0</v>
       </c>
-      <c r="C59" s="24">
+      <c r="C59" s="25">
         <f t="shared" si="1"/>
         <v>240</v>
       </c>
-      <c r="D59" s="24">
+      <c r="D59" s="25">
         <f t="shared" si="3"/>
         <v>5880</v>
       </c>
-      <c r="E59" s="25">
+      <c r="E59" s="26">
         <v>0.0</v>
       </c>
-      <c r="F59" s="27" t="b">
+      <c r="F59" s="28" t="b">
         <v>0</v>
       </c>
       <c r="G59" s="3"/>
@@ -3153,21 +3167,21 @@
     </row>
     <row r="60">
       <c r="A60" s="5"/>
-      <c r="B60" s="13">
+      <c r="B60" s="14">
         <v>49.0</v>
       </c>
-      <c r="C60" s="21">
+      <c r="C60" s="22">
         <f t="shared" si="1"/>
         <v>245</v>
       </c>
-      <c r="D60" s="21">
+      <c r="D60" s="22">
         <f t="shared" si="3"/>
         <v>6125</v>
       </c>
-      <c r="E60" s="14">
+      <c r="E60" s="15">
         <v>0.0</v>
       </c>
-      <c r="F60" s="22" t="b">
+      <c r="F60" s="23" t="b">
         <v>0</v>
       </c>
       <c r="G60" s="3"/>
@@ -3195,21 +3209,21 @@
     </row>
     <row r="61">
       <c r="A61" s="5"/>
-      <c r="B61" s="23">
+      <c r="B61" s="24">
         <v>50.0</v>
       </c>
-      <c r="C61" s="24">
+      <c r="C61" s="25">
         <f t="shared" si="1"/>
         <v>250</v>
       </c>
-      <c r="D61" s="24">
+      <c r="D61" s="25">
         <f t="shared" si="3"/>
         <v>6375</v>
       </c>
-      <c r="E61" s="25">
+      <c r="E61" s="26">
         <v>0.0</v>
       </c>
-      <c r="F61" s="27" t="b">
+      <c r="F61" s="28" t="b">
         <v>0</v>
       </c>
       <c r="G61" s="3"/>
@@ -3237,21 +3251,21 @@
     </row>
     <row r="62">
       <c r="A62" s="5"/>
-      <c r="B62" s="13">
+      <c r="B62" s="14">
         <v>51.0</v>
       </c>
-      <c r="C62" s="21">
+      <c r="C62" s="22">
         <f t="shared" si="1"/>
         <v>255</v>
       </c>
-      <c r="D62" s="21">
+      <c r="D62" s="22">
         <f t="shared" si="3"/>
         <v>6630</v>
       </c>
-      <c r="E62" s="14">
+      <c r="E62" s="15">
         <v>0.0</v>
       </c>
-      <c r="F62" s="22" t="b">
+      <c r="F62" s="23" t="b">
         <v>0</v>
       </c>
       <c r="G62" s="3"/>
@@ -3279,21 +3293,21 @@
     </row>
     <row r="63">
       <c r="A63" s="5"/>
-      <c r="B63" s="29">
+      <c r="B63" s="30">
         <v>52.0</v>
       </c>
-      <c r="C63" s="30">
+      <c r="C63" s="31">
         <f t="shared" si="1"/>
         <v>260</v>
       </c>
-      <c r="D63" s="30">
+      <c r="D63" s="31">
         <f t="shared" si="3"/>
         <v>6890</v>
       </c>
-      <c r="E63" s="31">
+      <c r="E63" s="32">
         <v>0.0</v>
       </c>
-      <c r="F63" s="32" t="b">
+      <c r="F63" s="33" t="b">
         <v>0</v>
       </c>
       <c r="G63" s="3"/>
@@ -31521,13 +31535,16 @@
     </row>
   </sheetData>
   <mergeCells count="5">
+    <mergeCell ref="B1:I1"/>
     <mergeCell ref="B3:D3"/>
+    <mergeCell ref="F3:G3"/>
     <mergeCell ref="B10:F10"/>
-    <mergeCell ref="F3:G3"/>
     <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B1:I1"/>
   </mergeCells>
-  <drawing r:id="rId4"/>
-  <legacyDrawing r:id="rId5"/>
+  <hyperlinks>
+    <hyperlink r:id="rId4" ref="K3"/>
+  </hyperlinks>
+  <drawing r:id="rId5"/>
+  <legacyDrawing r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>